<commit_message>
py model und reibung
</commit_message>
<xml_diff>
--- a/3DBeam/output/Querschnittswerte.xlsx
+++ b/3DBeam/output/Querschnittswerte.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,16 @@
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="15" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
+    <col width="15" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="15" customWidth="1" min="30" max="30"/>
+    <col width="15" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="15" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -535,25 +545,50 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>fvFek</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>rhok</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>E0mean</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>E90mean</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Furnierebene</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>rhok_Fe</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>G0mean</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>G4545</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>alpha</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>alphaT</t>
         </is>
@@ -585,18 +620,33 @@
         <v>2.5</v>
       </c>
       <c r="I2" t="n">
+        <v>31</v>
+      </c>
+      <c r="J2" t="n">
         <v>460</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>12000000000</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>370000000</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>735</v>
+      </c>
+      <c r="O2" t="n">
+        <v>500</v>
+      </c>
+      <c r="P2" t="n">
+        <v>4227</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0.02</v>
       </c>
-      <c r="M2" t="n">
+      <c r="R2" t="n">
         <v>4e-06</v>
       </c>
     </row>
@@ -637,7 +687,7 @@
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>U [m]</t>
+          <t>U_achse [m]</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
@@ -657,16 +707,16 @@
         <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>209.35</v>
+        <v>186.27</v>
       </c>
       <c r="E8" t="n">
-        <v>13.82</v>
+        <v>12.3</v>
       </c>
       <c r="F8" t="n">
         <v>34.56</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="9">
@@ -680,16 +730,16 @@
         <v>10.16</v>
       </c>
       <c r="D9" t="n">
-        <v>164.78</v>
+        <v>146.61</v>
       </c>
       <c r="E9" t="n">
-        <v>12.76</v>
+        <v>11.36</v>
       </c>
       <c r="F9" t="n">
         <v>31.9</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="10">
@@ -703,16 +753,16 @@
         <v>9.31</v>
       </c>
       <c r="D10" t="n">
-        <v>127.04</v>
+        <v>113.02</v>
       </c>
       <c r="E10" t="n">
-        <v>11.7</v>
+        <v>10.41</v>
       </c>
       <c r="F10" t="n">
         <v>29.25</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="11">
@@ -726,16 +776,16 @@
         <v>8.470000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>95.55</v>
+        <v>85</v>
       </c>
       <c r="E11" t="n">
-        <v>10.64</v>
+        <v>9.470000000000001</v>
       </c>
       <c r="F11" t="n">
         <v>26.6</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="12">
@@ -749,16 +799,16 @@
         <v>7.62</v>
       </c>
       <c r="D12" t="n">
-        <v>69.75</v>
+        <v>62.04</v>
       </c>
       <c r="E12" t="n">
-        <v>9.58</v>
+        <v>8.52</v>
       </c>
       <c r="F12" t="n">
         <v>23.95</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="13">
@@ -772,16 +822,16 @@
         <v>6.78</v>
       </c>
       <c r="D13" t="n">
-        <v>49.08</v>
+        <v>43.65</v>
       </c>
       <c r="E13" t="n">
-        <v>8.52</v>
+        <v>7.58</v>
       </c>
       <c r="F13" t="n">
         <v>21.29</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="14">
@@ -795,16 +845,16 @@
         <v>5.93</v>
       </c>
       <c r="D14" t="n">
-        <v>32.96</v>
+        <v>29.31</v>
       </c>
       <c r="E14" t="n">
-        <v>7.46</v>
+        <v>6.64</v>
       </c>
       <c r="F14" t="n">
         <v>18.64</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="15">
@@ -818,16 +868,16 @@
         <v>5.09</v>
       </c>
       <c r="D15" t="n">
-        <v>20.83</v>
+        <v>18.51</v>
       </c>
       <c r="E15" t="n">
-        <v>6.39</v>
+        <v>5.69</v>
       </c>
       <c r="F15" t="n">
         <v>15.99</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="16">
@@ -841,16 +891,16 @@
         <v>4.24</v>
       </c>
       <c r="D16" t="n">
-        <v>12.12</v>
+        <v>10.77</v>
       </c>
       <c r="E16" t="n">
-        <v>5.33</v>
+        <v>4.75</v>
       </c>
       <c r="F16" t="n">
         <v>13.33</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="17">
@@ -864,16 +914,16 @@
         <v>3.4</v>
       </c>
       <c r="D17" t="n">
-        <v>6.26</v>
+        <v>5.55</v>
       </c>
       <c r="E17" t="n">
-        <v>4.27</v>
+        <v>3.8</v>
       </c>
       <c r="F17" t="n">
         <v>10.68</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>